<commit_message>
Add a line attack command where all objects along a path get hit. No need to store list of targets on lightning command as they can be reloaded based on the path. Move historical command load state until after maps have been loaded for safety in case there's a future dependency on a command needing state from other properties not yet loaded. Fix compile error after getting latest GoRogue version. Separate player's basic attack from unarmed attack in preparation for equipping melee weapons.
</commit_message>
<xml_diff>
--- a/MarsUndiscovered/Spreadsheets/Breeds.xlsx
+++ b/MarsUndiscovered/Spreadsheets/Breeds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\MarsUndiscovered\MarsUndiscovered\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D211366-4BC2-44BC-A727-EB4502923AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CACBAD-25D8-44BE-8EE8-A4F02C3181C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{B3EDC88D-065E-48D2-99EE-6EE48DB38C44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B3EDC88D-065E-48D2-99EE-6EE48DB38C44}"/>
   </bookViews>
   <sheets>
     <sheet name="Breeds" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>MaxHealth</t>
+  </si>
+  <si>
+    <t>LineAttackMin</t>
+  </si>
+  <si>
+    <t>LineAttackMax</t>
   </si>
 </sst>
 </file>
@@ -457,25 +463,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6588FC-8195-4803-811E-22447E3C22B0}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="1" customWidth="1"/>
-    <col min="4" max="6" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="48.109375" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" style="1" customWidth="1"/>
+    <col min="4" max="6" width="28.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,8 +512,14 @@
       <c r="J1" t="s">
         <v>11</v>
       </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -533,7 +545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -559,7 +571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>

</xml_diff>